<commit_message>
Finished the summary statistics part
</commit_message>
<xml_diff>
--- a/SummaryStats.xlsx
+++ b/SummaryStats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF395EFF-78CB-4494-B9AC-A8383A475682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57684B7F-6CC0-45D2-9B0E-5C1D8C3F4132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="4530" windowWidth="9990" windowHeight="11385" xr2:uid="{057085EE-CEC8-486B-B428-B0EF905CE233}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{057085EE-CEC8-486B-B428-B0EF905CE233}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PerChange" sheetId="1" r:id="rId1"/>
+    <sheet name="PostChange" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Year</t>
   </si>
@@ -75,7 +76,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -148,7 +149,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -468,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA984DF-BD97-4467-88D7-E5141B768970}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,4 +624,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2936120B-C839-4C26-B848-2F90CAF4770E}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2016.86434734205</v>
+      </c>
+      <c r="C2" s="5">
+        <v>12279.756415251901</v>
+      </c>
+      <c r="D2" s="5">
+        <v>23363.6305037573</v>
+      </c>
+      <c r="E2" s="5">
+        <v>113.33453938213199</v>
+      </c>
+      <c r="F2" s="5">
+        <v>57.906991372112401</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1.3508266072919599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2017</v>
+      </c>
+      <c r="C3" s="6">
+        <v>11291</v>
+      </c>
+      <c r="D3" s="6">
+        <v>18243</v>
+      </c>
+      <c r="E3" s="6">
+        <v>145</v>
+      </c>
+      <c r="F3" s="1">
+        <v>58.9</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1996</v>
+      </c>
+      <c r="C4" s="1">
+        <v>495</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="8">
+        <v>54995</v>
+      </c>
+      <c r="D5" s="8">
+        <v>177644</v>
+      </c>
+      <c r="E5" s="1">
+        <v>580</v>
+      </c>
+      <c r="F5" s="1">
+        <v>201.8</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.0250657954429601</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4741.3826059297799</v>
+      </c>
+      <c r="D6" s="5">
+        <v>19472.1146895741</v>
+      </c>
+      <c r="E6" s="4">
+        <v>62.010438197644</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10.1259774204699</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.43237138391874302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>